<commit_message>
Update Scorecard - F1 values.xlsx
</commit_message>
<xml_diff>
--- a/Supervised_Learning/Scorecard - F1 values.xlsx
+++ b/Supervised_Learning/Scorecard - F1 values.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfred\Documents\GitHub\DSaML_Projects\Supervised_Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF8D7CF6-4FFF-4D39-B496-B8EB52D69314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3664BD6-4916-4D72-A749-C541733FCC0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{36C6B408-B3DB-4C98-8193-63E0F9F2EE8D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{36C6B408-B3DB-4C98-8193-63E0F9F2EE8D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Final" sheetId="2" r:id="rId2"/>
+    <sheet name="Snippet" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -187,7 +188,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="81">
   <si>
     <t>RoomType</t>
   </si>
@@ -401,6 +402,36 @@
   <si>
     <t>Baseline 3.0 - 14+1 Features</t>
   </si>
+  <si>
+    <t>Baseline 8</t>
+  </si>
+  <si>
+    <t>Baseline 10</t>
+  </si>
+  <si>
+    <t>Baseline 14+1</t>
+  </si>
+  <si>
+    <t>Gradient Boosting</t>
+  </si>
+  <si>
+    <t>Neural Networks</t>
+  </si>
+  <si>
+    <t>Extra Trees</t>
+  </si>
+  <si>
+    <t>F1-Train</t>
+  </si>
+  <si>
+    <t>F1-Validation</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>F1 delta</t>
+  </si>
 </sst>
 </file>
 
@@ -531,7 +562,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="38">
+  <borders count="46">
     <border>
       <left/>
       <right/>
@@ -1022,12 +1053,112 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="233">
+  <cellXfs count="259">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1470,33 +1601,6 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1631,10 +1735,109 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2088,15 +2291,15 @@
       <c r="AE1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AG1" s="176" t="s">
+      <c r="AG1" s="222" t="s">
         <v>27</v>
       </c>
-      <c r="AH1" s="177"/>
-      <c r="AI1" s="177"/>
-      <c r="AJ1" s="177"/>
-      <c r="AK1" s="177"/>
-      <c r="AL1" s="177"/>
-      <c r="AM1" s="178"/>
+      <c r="AH1" s="223"/>
+      <c r="AI1" s="223"/>
+      <c r="AJ1" s="223"/>
+      <c r="AK1" s="223"/>
+      <c r="AL1" s="223"/>
+      <c r="AM1" s="224"/>
     </row>
     <row r="2" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="18" t="s">
@@ -5299,8 +5502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E47D96A-367B-44D4-A207-423C8F54CE2A}">
   <dimension ref="A1:AZ39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AD20" sqref="AD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5359,10 +5562,10 @@
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
-      <c r="R1" s="227" t="s">
+      <c r="R1" s="218" t="s">
         <v>69</v>
       </c>
-      <c r="S1" s="228" t="s">
+      <c r="S1" s="219" t="s">
         <v>56</v>
       </c>
       <c r="T1" s="1"/>
@@ -5418,13 +5621,13 @@
       <c r="P2" s="120" t="s">
         <v>10</v>
       </c>
-      <c r="Q2" s="226" t="s">
+      <c r="Q2" s="217" t="s">
         <v>11</v>
       </c>
       <c r="R2" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="S2" s="229" t="s">
+      <c r="S2" s="220" t="s">
         <v>43</v>
       </c>
       <c r="T2" s="91" t="s">
@@ -5570,7 +5773,7 @@
       <c r="AZ3" s="51"/>
     </row>
     <row r="4" spans="1:52" x14ac:dyDescent="0.3">
-      <c r="A4" s="182" t="s">
+      <c r="A4" s="230" t="s">
         <v>49</v>
       </c>
       <c r="B4" s="113" t="s">
@@ -5660,42 +5863,42 @@
       <c r="AL4" s="72"/>
       <c r="AM4" s="96"/>
       <c r="AN4" s="56"/>
-      <c r="AO4" s="192">
+      <c r="AO4" s="183">
         <f>1-Y4/X4</f>
         <v>1.2610340479193294E-3</v>
       </c>
-      <c r="AP4" s="193">
+      <c r="AP4" s="184">
         <f>1-AA4/Z4</f>
         <v>4.2998897464167629E-2</v>
       </c>
-      <c r="AQ4" s="193">
+      <c r="AQ4" s="184">
         <f>1-AC4/AB4</f>
         <v>7.4152542372881269E-2</v>
       </c>
-      <c r="AR4" s="193">
+      <c r="AR4" s="184">
         <f>1-AE4/AD4</f>
         <v>3.5106382978723372E-2</v>
       </c>
-      <c r="AS4" s="193">
+      <c r="AS4" s="184">
         <f>1-AG4/AF4</f>
         <v>2.4968789013732895E-3</v>
       </c>
-      <c r="AT4" s="193">
+      <c r="AT4" s="184">
         <f>1-AI4/AH4</f>
         <v>3.0949839914621191E-2</v>
       </c>
-      <c r="AU4" s="194">
+      <c r="AU4" s="185">
         <f>1-AK4/AJ4</f>
         <v>3.4482758620689724E-2</v>
       </c>
-      <c r="AV4" s="208"/>
+      <c r="AV4" s="199"/>
       <c r="AW4" s="51"/>
       <c r="AX4" s="51"/>
       <c r="AY4" s="51"/>
       <c r="AZ4" s="51"/>
     </row>
     <row r="5" spans="1:52" x14ac:dyDescent="0.3">
-      <c r="A5" s="183"/>
+      <c r="A5" s="231"/>
       <c r="B5" s="99" t="s">
         <v>52</v>
       </c>
@@ -5781,42 +5984,42 @@
       <c r="AL5" s="72"/>
       <c r="AM5" s="96"/>
       <c r="AN5" s="56"/>
-      <c r="AO5" s="195">
+      <c r="AO5" s="186">
         <f t="shared" ref="AO5:AO8" si="0">1-Y5/X5</f>
         <v>0</v>
       </c>
-      <c r="AP5" s="191">
+      <c r="AP5" s="182">
         <f t="shared" ref="AP5:AP8" si="1">1-AA5/Z5</f>
         <v>2.6402640264026389E-2</v>
       </c>
-      <c r="AQ5" s="191">
+      <c r="AQ5" s="182">
         <f t="shared" ref="AQ5:AQ8" si="2">1-AC5/AB5</f>
         <v>2.5274725274725296E-2</v>
       </c>
-      <c r="AR5" s="191">
+      <c r="AR5" s="182">
         <f t="shared" ref="AR5:AR8" si="3">1-AE5/AD5</f>
         <v>2.2678185745140356E-2</v>
       </c>
-      <c r="AS5" s="191">
+      <c r="AS5" s="182">
         <f>MAX(1-AG5/AF5,0)</f>
         <v>0</v>
       </c>
-      <c r="AT5" s="191">
+      <c r="AT5" s="182">
         <f t="shared" ref="AT5:AT8" si="4">1-AI5/AH5</f>
         <v>1.413043478260867E-2</v>
       </c>
-      <c r="AU5" s="196">
+      <c r="AU5" s="187">
         <f t="shared" ref="AU5:AU8" si="5">1-AK5/AJ5</f>
         <v>1.2048192771084376E-2</v>
       </c>
-      <c r="AV5" s="208"/>
+      <c r="AV5" s="199"/>
       <c r="AW5" s="51"/>
       <c r="AX5" s="51"/>
       <c r="AY5" s="51"/>
       <c r="AZ5" s="51"/>
     </row>
     <row r="6" spans="1:52" x14ac:dyDescent="0.3">
-      <c r="A6" s="183"/>
+      <c r="A6" s="231"/>
       <c r="B6" s="99" t="s">
         <v>58</v>
       </c>
@@ -5869,10 +6072,10 @@
       <c r="W6" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="X6" s="214">
+      <c r="X6" s="205">
         <v>0.81100000000000005</v>
       </c>
-      <c r="Y6" s="213">
+      <c r="Y6" s="204">
         <v>0.80900000000000005</v>
       </c>
       <c r="Z6" s="71">
@@ -5893,10 +6096,10 @@
       <c r="AE6" s="71">
         <v>0.92500000000000004</v>
       </c>
-      <c r="AF6" s="188">
+      <c r="AF6" s="179">
         <v>0.81799999999999995</v>
       </c>
-      <c r="AG6" s="188">
+      <c r="AG6" s="179">
         <v>0.81599999999999995</v>
       </c>
       <c r="AH6" s="170">
@@ -5914,42 +6117,42 @@
       <c r="AL6" s="90"/>
       <c r="AM6" s="93"/>
       <c r="AN6" s="51"/>
-      <c r="AO6" s="195">
+      <c r="AO6" s="186">
         <f t="shared" si="0"/>
         <v>2.4660912453761119E-3</v>
       </c>
-      <c r="AP6" s="191">
+      <c r="AP6" s="182">
         <f t="shared" si="1"/>
         <v>3.6105032822757122E-2</v>
       </c>
-      <c r="AQ6" s="191">
+      <c r="AQ6" s="182">
         <f t="shared" si="2"/>
         <v>9.2975206611570216E-2</v>
       </c>
-      <c r="AR6" s="191">
+      <c r="AR6" s="182">
         <f t="shared" si="3"/>
         <v>5.0308008213552302E-2</v>
       </c>
-      <c r="AS6" s="191">
+      <c r="AS6" s="182">
         <f t="shared" ref="AS6:AS8" si="6">1-AG6/AF6</f>
         <v>2.4449877750610804E-3</v>
       </c>
-      <c r="AT6" s="225">
+      <c r="AT6" s="216">
         <f t="shared" si="4"/>
         <v>4.6986721144024468E-2</v>
       </c>
-      <c r="AU6" s="196">
+      <c r="AU6" s="187">
         <f t="shared" si="5"/>
         <v>5.0672182006204713E-2</v>
       </c>
-      <c r="AV6" s="208"/>
+      <c r="AV6" s="199"/>
       <c r="AW6" s="51"/>
       <c r="AX6" s="51"/>
       <c r="AY6" s="51"/>
       <c r="AZ6" s="51"/>
     </row>
     <row r="7" spans="1:52" x14ac:dyDescent="0.3">
-      <c r="A7" s="183"/>
+      <c r="A7" s="231"/>
       <c r="B7" s="99" t="s">
         <v>59</v>
       </c>
@@ -6004,16 +6207,16 @@
       <c r="Y7" s="71">
         <v>0.80700000000000005</v>
       </c>
-      <c r="Z7" s="213">
+      <c r="Z7" s="204">
         <v>0.92400000000000004</v>
       </c>
-      <c r="AA7" s="213">
+      <c r="AA7" s="204">
         <v>0.89500000000000002</v>
       </c>
-      <c r="AB7" s="213">
+      <c r="AB7" s="204">
         <v>0.96599999999999997</v>
       </c>
-      <c r="AC7" s="213">
+      <c r="AC7" s="204">
         <v>0.88500000000000001</v>
       </c>
       <c r="AD7" s="170">
@@ -6022,10 +6225,10 @@
       <c r="AE7" s="170">
         <v>0.92800000000000005</v>
       </c>
-      <c r="AF7" s="213">
+      <c r="AF7" s="204">
         <v>0.81699999999999995</v>
       </c>
-      <c r="AG7" s="213">
+      <c r="AG7" s="204">
         <v>0.81599999999999995</v>
       </c>
       <c r="AH7" s="71">
@@ -6043,42 +6246,42 @@
       <c r="AL7" s="90"/>
       <c r="AM7" s="93"/>
       <c r="AN7" s="51"/>
-      <c r="AO7" s="195">
+      <c r="AO7" s="186">
         <f t="shared" si="0"/>
         <v>2.4721878862793423E-3</v>
       </c>
-      <c r="AP7" s="191">
+      <c r="AP7" s="182">
         <f t="shared" si="1"/>
         <v>3.1385281385281405E-2</v>
       </c>
-      <c r="AQ7" s="191">
+      <c r="AQ7" s="182">
         <f t="shared" si="2"/>
         <v>8.3850931677018625E-2</v>
       </c>
-      <c r="AR7" s="225">
+      <c r="AR7" s="216">
         <f t="shared" si="3"/>
         <v>4.3298969072164906E-2</v>
       </c>
-      <c r="AS7" s="191">
+      <c r="AS7" s="182">
         <f t="shared" si="6"/>
         <v>1.223990208078285E-3</v>
       </c>
-      <c r="AT7" s="191">
+      <c r="AT7" s="182">
         <f t="shared" si="4"/>
         <v>4.2181069958847628E-2</v>
       </c>
-      <c r="AU7" s="196">
+      <c r="AU7" s="187">
         <f t="shared" si="5"/>
         <v>2.2151898734177111E-2</v>
       </c>
-      <c r="AV7" s="208"/>
+      <c r="AV7" s="199"/>
       <c r="AW7" s="51"/>
       <c r="AX7" s="51"/>
       <c r="AY7" s="51"/>
       <c r="AZ7" s="51"/>
     </row>
     <row r="8" spans="1:52" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="184"/>
+      <c r="A8" s="232"/>
       <c r="B8" s="101" t="s">
         <v>60</v>
       </c>
@@ -6159,10 +6362,10 @@
       <c r="AG8" s="79">
         <v>0.81399999999999995</v>
       </c>
-      <c r="AH8" s="212">
+      <c r="AH8" s="203">
         <v>0.97299999999999998</v>
       </c>
-      <c r="AI8" s="212">
+      <c r="AI8" s="203">
         <v>0.93200000000000005</v>
       </c>
       <c r="AJ8" s="174">
@@ -6174,35 +6377,35 @@
       <c r="AL8" s="90"/>
       <c r="AM8" s="93"/>
       <c r="AN8" s="51"/>
-      <c r="AO8" s="197">
+      <c r="AO8" s="188">
         <f t="shared" si="0"/>
         <v>1.2345679012345512E-3</v>
       </c>
-      <c r="AP8" s="198">
+      <c r="AP8" s="189">
         <f t="shared" si="1"/>
         <v>3.2608695652173947E-2</v>
       </c>
-      <c r="AQ8" s="198">
+      <c r="AQ8" s="189">
         <f t="shared" si="2"/>
         <v>9.213250517598337E-2</v>
       </c>
-      <c r="AR8" s="198">
+      <c r="AR8" s="189">
         <f t="shared" si="3"/>
         <v>4.9382716049382602E-2</v>
       </c>
-      <c r="AS8" s="198">
+      <c r="AS8" s="189">
         <f t="shared" si="6"/>
         <v>2.450980392156854E-3</v>
       </c>
-      <c r="AT8" s="198">
+      <c r="AT8" s="189">
         <f t="shared" si="4"/>
         <v>4.2137718396711099E-2</v>
       </c>
-      <c r="AU8" s="223">
+      <c r="AU8" s="214">
         <f t="shared" si="5"/>
         <v>2.9442691903259655E-2</v>
       </c>
-      <c r="AV8" s="208"/>
+      <c r="AV8" s="199"/>
       <c r="AW8" s="51"/>
       <c r="AX8" s="51"/>
       <c r="AY8" s="51"/>
@@ -6249,21 +6452,21 @@
       <c r="AL9" s="72"/>
       <c r="AM9" s="96"/>
       <c r="AN9" s="56"/>
-      <c r="AO9" s="209"/>
+      <c r="AO9" s="200"/>
       <c r="AP9" s="167"/>
       <c r="AQ9" s="167"/>
       <c r="AR9" s="167"/>
       <c r="AS9" s="167"/>
       <c r="AT9" s="167"/>
       <c r="AU9" s="167"/>
-      <c r="AV9" s="208"/>
+      <c r="AV9" s="199"/>
       <c r="AW9" s="51"/>
       <c r="AX9" s="51"/>
       <c r="AY9" s="51"/>
       <c r="AZ9" s="51"/>
     </row>
     <row r="10" spans="1:52" s="51" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="179" t="s">
+      <c r="A10" s="225" t="s">
         <v>50</v>
       </c>
       <c r="B10" s="113" t="s">
@@ -6330,10 +6533,10 @@
       </c>
       <c r="AF10" s="72"/>
       <c r="AG10" s="72"/>
-      <c r="AH10" s="215">
+      <c r="AH10" s="206">
         <v>0.91200000000000003</v>
       </c>
-      <c r="AI10" s="216">
+      <c r="AI10" s="207">
         <v>0.90800000000000003</v>
       </c>
       <c r="AJ10" s="60">
@@ -6345,26 +6548,26 @@
       <c r="AL10" s="72"/>
       <c r="AM10" s="96"/>
       <c r="AN10" s="56"/>
-      <c r="AO10" s="209"/>
+      <c r="AO10" s="200"/>
       <c r="AP10" s="167"/>
       <c r="AQ10" s="167"/>
-      <c r="AR10" s="199">
+      <c r="AR10" s="190">
         <f>1-AE10/AD10</f>
         <v>7.5150300601202313E-2</v>
       </c>
       <c r="AS10" s="167"/>
-      <c r="AT10" s="202">
+      <c r="AT10" s="193">
         <f>1-AI10/AH10</f>
         <v>4.3859649122807154E-3</v>
       </c>
-      <c r="AU10" s="203">
+      <c r="AU10" s="194">
         <f>1-AK10/AJ10</f>
         <v>1.0764262648008671E-2</v>
       </c>
-      <c r="AV10" s="208"/>
+      <c r="AV10" s="199"/>
     </row>
     <row r="11" spans="1:52" s="51" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="180"/>
+      <c r="A11" s="226"/>
       <c r="B11" s="99" t="s">
         <v>54</v>
       </c>
@@ -6440,26 +6643,26 @@
       <c r="AL11" s="72"/>
       <c r="AM11" s="96"/>
       <c r="AN11" s="56"/>
-      <c r="AO11" s="209"/>
+      <c r="AO11" s="200"/>
       <c r="AP11" s="167"/>
       <c r="AQ11" s="167"/>
-      <c r="AR11" s="200">
+      <c r="AR11" s="191">
         <f t="shared" ref="AR11:AR16" si="7">1-AE11/AD11</f>
         <v>6.1287027579162379E-2</v>
       </c>
       <c r="AS11" s="167"/>
-      <c r="AT11" s="204">
+      <c r="AT11" s="195">
         <f t="shared" ref="AT11:AT16" si="8">1-AI11/AH11</f>
         <v>2.2026431718061845E-3</v>
       </c>
-      <c r="AU11" s="205">
+      <c r="AU11" s="196">
         <f t="shared" ref="AU11:AU16" si="9">1-AK11/AJ11</f>
         <v>8.6580086580086979E-3</v>
       </c>
-      <c r="AV11" s="208"/>
+      <c r="AV11" s="199"/>
     </row>
     <row r="12" spans="1:52" s="51" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="180"/>
+      <c r="A12" s="226"/>
       <c r="B12" s="99" t="s">
         <v>55</v>
       </c>
@@ -6524,35 +6727,35 @@
       <c r="AI12" s="68">
         <v>0.90400000000000003</v>
       </c>
-      <c r="AJ12" s="217">
+      <c r="AJ12" s="208">
         <v>0.92700000000000005</v>
       </c>
-      <c r="AK12" s="218">
+      <c r="AK12" s="209">
         <v>0.92</v>
       </c>
       <c r="AL12" s="72"/>
       <c r="AM12" s="96"/>
       <c r="AN12" s="56"/>
-      <c r="AO12" s="209"/>
+      <c r="AO12" s="200"/>
       <c r="AP12" s="167"/>
       <c r="AQ12" s="167"/>
-      <c r="AR12" s="200">
+      <c r="AR12" s="191">
         <f t="shared" si="7"/>
         <v>5.7435897435897387E-2</v>
       </c>
       <c r="AS12" s="167"/>
-      <c r="AT12" s="204">
+      <c r="AT12" s="195">
         <f t="shared" si="8"/>
         <v>3.3076074972436809E-3</v>
       </c>
-      <c r="AU12" s="205">
+      <c r="AU12" s="196">
         <f t="shared" si="9"/>
         <v>7.5512405609493571E-3</v>
       </c>
-      <c r="AV12" s="208"/>
+      <c r="AV12" s="199"/>
     </row>
     <row r="13" spans="1:52" s="51" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="180"/>
+      <c r="A13" s="226"/>
       <c r="B13" s="99" t="s">
         <v>61</v>
       </c>
@@ -6628,26 +6831,26 @@
       <c r="AL13" s="72"/>
       <c r="AM13" s="96"/>
       <c r="AN13" s="56"/>
-      <c r="AO13" s="209"/>
+      <c r="AO13" s="200"/>
       <c r="AP13" s="167"/>
       <c r="AQ13" s="167"/>
-      <c r="AR13" s="200">
+      <c r="AR13" s="191">
         <f t="shared" si="7"/>
         <v>6.8825910931174072E-2</v>
       </c>
       <c r="AS13" s="167"/>
-      <c r="AT13" s="204">
+      <c r="AT13" s="195">
         <f t="shared" si="8"/>
         <v>5.5005500550054931E-3</v>
       </c>
-      <c r="AU13" s="205">
+      <c r="AU13" s="196">
         <f t="shared" si="9"/>
         <v>9.7087378640776656E-3</v>
       </c>
-      <c r="AV13" s="208"/>
+      <c r="AV13" s="199"/>
     </row>
     <row r="14" spans="1:52" s="51" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="180"/>
+      <c r="A14" s="226"/>
       <c r="B14" s="99" t="s">
         <v>62</v>
       </c>
@@ -6723,26 +6926,26 @@
       <c r="AL14" s="72"/>
       <c r="AM14" s="96"/>
       <c r="AN14" s="56"/>
-      <c r="AO14" s="209"/>
+      <c r="AO14" s="200"/>
       <c r="AP14" s="167"/>
       <c r="AQ14" s="167"/>
-      <c r="AR14" s="200">
+      <c r="AR14" s="191">
         <f t="shared" si="7"/>
         <v>6.7676767676767668E-2</v>
       </c>
       <c r="AS14" s="167"/>
-      <c r="AT14" s="204">
+      <c r="AT14" s="195">
         <f t="shared" si="8"/>
         <v>4.3907793633369829E-3</v>
       </c>
-      <c r="AU14" s="205">
+      <c r="AU14" s="196">
         <f t="shared" si="9"/>
         <v>9.6982758620689502E-3</v>
       </c>
-      <c r="AV14" s="208"/>
+      <c r="AV14" s="199"/>
     </row>
     <row r="15" spans="1:52" s="51" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="180"/>
+      <c r="A15" s="226"/>
       <c r="B15" s="99" t="s">
         <v>63</v>
       </c>
@@ -6816,26 +7019,26 @@
       <c r="AL15" s="72"/>
       <c r="AM15" s="96"/>
       <c r="AN15" s="56"/>
-      <c r="AO15" s="209"/>
+      <c r="AO15" s="200"/>
       <c r="AP15" s="167"/>
       <c r="AQ15" s="167"/>
-      <c r="AR15" s="200">
+      <c r="AR15" s="191">
         <f t="shared" si="7"/>
         <v>5.7851239669421406E-2</v>
       </c>
       <c r="AS15" s="167"/>
-      <c r="AT15" s="204">
+      <c r="AT15" s="195">
         <f t="shared" si="8"/>
         <v>4.4296788482834915E-3</v>
       </c>
-      <c r="AU15" s="205">
+      <c r="AU15" s="196">
         <f t="shared" si="9"/>
         <v>1.0940919037199182E-2</v>
       </c>
-      <c r="AV15" s="208"/>
+      <c r="AV15" s="199"/>
     </row>
     <row r="16" spans="1:52" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="181"/>
+      <c r="A16" s="227"/>
       <c r="B16" s="101" t="s">
         <v>64</v>
       </c>
@@ -6882,10 +7085,10 @@
       <c r="AA16" s="90"/>
       <c r="AB16" s="90"/>
       <c r="AC16" s="90"/>
-      <c r="AD16" s="219">
+      <c r="AD16" s="210">
         <v>0.93200000000000005</v>
       </c>
-      <c r="AE16" s="220">
+      <c r="AE16" s="211">
         <v>0.90700000000000003</v>
       </c>
       <c r="AF16" s="72"/>
@@ -6905,23 +7108,23 @@
       <c r="AL16" s="90"/>
       <c r="AM16" s="93"/>
       <c r="AN16" s="51"/>
-      <c r="AO16" s="209"/>
+      <c r="AO16" s="200"/>
       <c r="AP16" s="167"/>
       <c r="AQ16" s="167"/>
-      <c r="AR16" s="201">
+      <c r="AR16" s="192">
         <f t="shared" si="7"/>
         <v>2.6824034334763991E-2</v>
       </c>
       <c r="AS16" s="167"/>
-      <c r="AT16" s="206">
+      <c r="AT16" s="197">
         <f t="shared" si="8"/>
         <v>1.1198208286674616E-3</v>
       </c>
-      <c r="AU16" s="207">
+      <c r="AU16" s="198">
         <f t="shared" si="9"/>
         <v>5.5370985603543366E-3</v>
       </c>
-      <c r="AV16" s="208"/>
+      <c r="AV16" s="199"/>
       <c r="AW16" s="51"/>
       <c r="AX16" s="51"/>
       <c r="AY16" s="51"/>
@@ -6968,14 +7171,14 @@
       <c r="AL17" s="72"/>
       <c r="AM17" s="96"/>
       <c r="AN17" s="56"/>
-      <c r="AO17" s="209"/>
+      <c r="AO17" s="200"/>
       <c r="AP17" s="167"/>
       <c r="AQ17" s="167"/>
       <c r="AR17" s="167"/>
       <c r="AS17" s="167"/>
       <c r="AT17" s="167"/>
       <c r="AU17" s="167"/>
-      <c r="AV17" s="208"/>
+      <c r="AV17" s="199"/>
       <c r="AW17" s="51"/>
       <c r="AX17" s="51"/>
       <c r="AY17" s="51"/>
@@ -7037,7 +7240,7 @@
       </c>
       <c r="AF18" s="72"/>
       <c r="AG18" s="72"/>
-      <c r="AH18" s="221">
+      <c r="AH18" s="212">
         <v>0.92200000000000004</v>
       </c>
       <c r="AI18" s="173">
@@ -7052,7 +7255,7 @@
       <c r="AL18" s="72"/>
       <c r="AM18" s="96"/>
       <c r="AN18" s="56"/>
-      <c r="AO18" s="209"/>
+      <c r="AO18" s="200"/>
       <c r="AP18" s="167"/>
       <c r="AQ18" s="167"/>
       <c r="AR18" s="166">
@@ -7068,7 +7271,7 @@
         <f>1-AK18/AJ18</f>
         <v>1.6322089227421177E-2</v>
       </c>
-      <c r="AV18" s="208"/>
+      <c r="AV18" s="199"/>
       <c r="AW18" s="51"/>
       <c r="AX18" s="51"/>
       <c r="AY18" s="51"/>
@@ -7115,14 +7318,14 @@
       <c r="AL19" s="72"/>
       <c r="AM19" s="96"/>
       <c r="AN19" s="56"/>
-      <c r="AO19" s="209"/>
+      <c r="AO19" s="200"/>
       <c r="AP19" s="167"/>
       <c r="AQ19" s="167"/>
       <c r="AR19" s="167"/>
       <c r="AS19" s="167"/>
       <c r="AT19" s="167"/>
       <c r="AU19" s="167"/>
-      <c r="AV19" s="208"/>
+      <c r="AV19" s="199"/>
       <c r="AW19" s="51"/>
       <c r="AX19" s="51"/>
       <c r="AY19" s="51"/>
@@ -7205,23 +7408,23 @@
       <c r="AL20" s="72"/>
       <c r="AM20" s="96"/>
       <c r="AN20" s="56"/>
-      <c r="AO20" s="209"/>
+      <c r="AO20" s="200"/>
       <c r="AP20" s="167"/>
       <c r="AQ20" s="167"/>
-      <c r="AR20" s="199">
+      <c r="AR20" s="190">
         <f>1-AE20/AD20</f>
         <v>4.658385093167694E-2</v>
       </c>
       <c r="AS20" s="167"/>
-      <c r="AT20" s="224">
+      <c r="AT20" s="215">
         <f>1-AI20/AH20</f>
         <v>2.9288702928870203E-2</v>
       </c>
-      <c r="AU20" s="203">
+      <c r="AU20" s="194">
         <f>1-AK20/AJ20</f>
         <v>1.1714589989350266E-2</v>
       </c>
-      <c r="AV20" s="208"/>
+      <c r="AV20" s="199"/>
       <c r="AW20" s="51"/>
       <c r="AX20" s="51"/>
       <c r="AY20" s="51"/>
@@ -7302,23 +7505,23 @@
       <c r="AL21" s="72"/>
       <c r="AM21" s="96"/>
       <c r="AN21" s="56"/>
-      <c r="AO21" s="209"/>
+      <c r="AO21" s="200"/>
       <c r="AP21" s="167"/>
       <c r="AQ21" s="167"/>
-      <c r="AR21" s="201">
+      <c r="AR21" s="192">
         <f>1-AE21/AD21</f>
         <v>7.0103092783505128E-2</v>
       </c>
       <c r="AS21" s="167"/>
-      <c r="AT21" s="206">
+      <c r="AT21" s="197">
         <f>1-AI21/AH21</f>
         <v>4.4742729306487261E-3</v>
       </c>
-      <c r="AU21" s="223">
+      <c r="AU21" s="214">
         <f>1-AK21/AJ21</f>
         <v>7.6754385964912242E-3</v>
       </c>
-      <c r="AV21" s="208"/>
+      <c r="AV21" s="199"/>
       <c r="AW21" s="51"/>
       <c r="AX21" s="51"/>
       <c r="AY21" s="51"/>
@@ -7365,14 +7568,14 @@
       <c r="AL22" s="72"/>
       <c r="AM22" s="96"/>
       <c r="AN22" s="56"/>
-      <c r="AO22" s="209"/>
+      <c r="AO22" s="200"/>
       <c r="AP22" s="167"/>
       <c r="AQ22" s="167"/>
       <c r="AR22" s="167"/>
       <c r="AS22" s="167"/>
       <c r="AT22" s="167"/>
       <c r="AU22" s="167"/>
-      <c r="AV22" s="208"/>
+      <c r="AV22" s="199"/>
       <c r="AW22" s="51"/>
       <c r="AX22" s="51"/>
       <c r="AY22" s="51"/>
@@ -7425,7 +7628,7 @@
         <v>20</v>
       </c>
       <c r="R23" s="145"/>
-      <c r="S23" s="230" t="s">
+      <c r="S23" s="221" t="s">
         <v>20</v>
       </c>
       <c r="T23" s="144" t="s">
@@ -7448,30 +7651,30 @@
       <c r="AG23" s="80"/>
       <c r="AH23" s="80"/>
       <c r="AI23" s="80"/>
-      <c r="AJ23" s="186">
+      <c r="AJ23" s="177">
         <v>0.96</v>
       </c>
-      <c r="AK23" s="187">
+      <c r="AK23" s="178">
         <v>0.93</v>
       </c>
       <c r="AL23" s="172">
         <v>0.98899999999999999</v>
       </c>
-      <c r="AM23" s="185">
+      <c r="AM23" s="176">
         <v>0.94099999999999995</v>
       </c>
       <c r="AN23" s="56"/>
-      <c r="AO23" s="210"/>
-      <c r="AP23" s="211"/>
-      <c r="AQ23" s="211"/>
-      <c r="AR23" s="211"/>
-      <c r="AS23" s="211"/>
-      <c r="AT23" s="211"/>
+      <c r="AO23" s="201"/>
+      <c r="AP23" s="202"/>
+      <c r="AQ23" s="202"/>
+      <c r="AR23" s="202"/>
+      <c r="AS23" s="202"/>
+      <c r="AT23" s="202"/>
       <c r="AU23" s="168">
         <f>1-AK23/AJ23</f>
         <v>3.1249999999999889E-2</v>
       </c>
-      <c r="AV23" s="222">
+      <c r="AV23" s="213">
         <f>1-AM23/AL23</f>
         <v>4.8533872598584438E-2</v>
       </c>
@@ -7497,10 +7700,10 @@
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
       <c r="Q24" s="4"/>
-      <c r="R24" s="231" t="s">
+      <c r="R24" s="228" t="s">
         <v>57</v>
       </c>
-      <c r="S24" s="232"/>
+      <c r="S24" s="229"/>
       <c r="T24" s="4"/>
       <c r="U24" s="4"/>
       <c r="V24" s="4"/>
@@ -7522,14 +7725,14 @@
       <c r="AL24" s="4"/>
       <c r="AM24" s="4"/>
       <c r="AN24" s="56"/>
-      <c r="AO24" s="189"/>
-      <c r="AP24" s="189"/>
-      <c r="AQ24" s="189"/>
-      <c r="AR24" s="189"/>
-      <c r="AS24" s="189"/>
-      <c r="AT24" s="189"/>
-      <c r="AU24" s="189"/>
-      <c r="AV24" s="189"/>
+      <c r="AO24" s="180"/>
+      <c r="AP24" s="180"/>
+      <c r="AQ24" s="180"/>
+      <c r="AR24" s="180"/>
+      <c r="AS24" s="180"/>
+      <c r="AT24" s="180"/>
+      <c r="AU24" s="180"/>
+      <c r="AV24" s="180"/>
       <c r="AW24" s="4"/>
     </row>
     <row r="25" spans="1:52" x14ac:dyDescent="0.3">
@@ -7572,16 +7775,16 @@
       <c r="AL25" s="4"/>
       <c r="AM25" s="16"/>
       <c r="AN25" s="56"/>
-      <c r="AR25" s="190">
+      <c r="AR25" s="181">
         <f>+AR10-AR16</f>
         <v>4.8326266266438322E-2</v>
       </c>
-      <c r="AS25" s="190"/>
-      <c r="AT25" s="190">
+      <c r="AS25" s="181"/>
+      <c r="AT25" s="181">
         <f>+AT10-AT16</f>
         <v>3.2661440836132538E-3</v>
       </c>
-      <c r="AU25" s="190">
+      <c r="AU25" s="181">
         <f>+AU10-AU16</f>
         <v>5.2271640876543346E-3</v>
       </c>
@@ -7616,45 +7819,45 @@
       <c r="AA26" s="4"/>
       <c r="AB26" s="4"/>
       <c r="AC26" s="4"/>
-      <c r="AD26" s="190">
+      <c r="AD26" s="181">
         <f>+AD18-AD16</f>
         <v>-1.0000000000000009E-2</v>
       </c>
-      <c r="AE26" s="190">
+      <c r="AE26" s="181">
         <f>+AE18-AE16</f>
         <v>1.0000000000000009E-3</v>
       </c>
       <c r="AF26" s="4"/>
       <c r="AG26" s="4"/>
-      <c r="AH26" s="190">
+      <c r="AH26" s="181">
         <f>+AH18-AH16</f>
         <v>2.9000000000000026E-2</v>
       </c>
-      <c r="AI26" s="190">
+      <c r="AI26" s="181">
         <f>+AI18-AI16</f>
         <v>1.8000000000000016E-2</v>
       </c>
-      <c r="AJ26" s="190">
+      <c r="AJ26" s="181">
         <f>+AJ18-AJ16</f>
         <v>1.6000000000000014E-2</v>
       </c>
-      <c r="AK26" s="190">
+      <c r="AK26" s="181">
         <f>+AK18-AK16</f>
         <v>6.0000000000000053E-3</v>
       </c>
       <c r="AL26" s="4"/>
       <c r="AM26" s="4"/>
       <c r="AN26" s="56"/>
-      <c r="AR26" s="190">
+      <c r="AR26" s="181">
         <f>+AR18-AR16</f>
         <v>-1.1639652556022062E-2</v>
       </c>
-      <c r="AS26" s="190"/>
-      <c r="AT26" s="190">
+      <c r="AS26" s="181"/>
+      <c r="AT26" s="181">
         <f>+AT18-AT16</f>
         <v>1.1895363553111271E-2</v>
       </c>
-      <c r="AU26" s="190">
+      <c r="AU26" s="181">
         <f>+AU18-AU16</f>
         <v>1.0784990667066841E-2</v>
       </c>
@@ -8202,4 +8405,236 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AC22DC2-0CF8-474B-B849-F9774C5DDF03}">
+  <dimension ref="C2:L8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="D3" s="236" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="254"/>
+      <c r="F3" s="237"/>
+      <c r="G3" s="236" t="s">
+        <v>72</v>
+      </c>
+      <c r="H3" s="254"/>
+      <c r="I3" s="237"/>
+      <c r="J3" s="254" t="s">
+        <v>73</v>
+      </c>
+      <c r="K3" s="254"/>
+      <c r="L3" s="237"/>
+    </row>
+    <row r="4" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D4" s="238" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" s="239" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4" s="240" t="s">
+        <v>80</v>
+      </c>
+      <c r="G4" s="238" t="s">
+        <v>77</v>
+      </c>
+      <c r="H4" s="239" t="s">
+        <v>78</v>
+      </c>
+      <c r="I4" s="240" t="s">
+        <v>80</v>
+      </c>
+      <c r="J4" s="255" t="s">
+        <v>77</v>
+      </c>
+      <c r="K4" s="239" t="s">
+        <v>78</v>
+      </c>
+      <c r="L4" s="240" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C5" s="233" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="241">
+        <f>+Final!AD18</f>
+        <v>0.92200000000000004</v>
+      </c>
+      <c r="E5" s="242">
+        <f>+Final!AE18</f>
+        <v>0.90800000000000003</v>
+      </c>
+      <c r="F5" s="243">
+        <f>1-(+E5/D5)</f>
+        <v>1.5184381778741929E-2</v>
+      </c>
+      <c r="G5" s="241">
+        <f>+Final!AD20</f>
+        <v>0.96599999999999997</v>
+      </c>
+      <c r="H5" s="242">
+        <f>+Final!AE20</f>
+        <v>0.92100000000000004</v>
+      </c>
+      <c r="I5" s="243">
+        <f>1-(+H5/G5)</f>
+        <v>4.658385093167694E-2</v>
+      </c>
+      <c r="J5" s="241" t="s">
+        <v>79</v>
+      </c>
+      <c r="K5" s="242" t="s">
+        <v>79</v>
+      </c>
+      <c r="L5" s="243" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C6" s="234" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="250">
+        <f>+Final!AH18</f>
+        <v>0.92200000000000004</v>
+      </c>
+      <c r="E6" s="251">
+        <f>+Final!AI18</f>
+        <v>0.91</v>
+      </c>
+      <c r="F6" s="256">
+        <f t="shared" ref="F6:F8" si="0">1-(+E6/D6)</f>
+        <v>1.3015184381778733E-2</v>
+      </c>
+      <c r="G6" s="244">
+        <f>+Final!AH20</f>
+        <v>0.95599999999999996</v>
+      </c>
+      <c r="H6" s="245">
+        <f>+Final!AI20</f>
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="I6" s="258">
+        <f t="shared" ref="I6" si="1">1-(+H6/G6)</f>
+        <v>2.9288702928870203E-2</v>
+      </c>
+      <c r="J6" s="244" t="s">
+        <v>79</v>
+      </c>
+      <c r="K6" s="245" t="s">
+        <v>79</v>
+      </c>
+      <c r="L6" s="258" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C7" s="234" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="244">
+        <f>+Final!AJ18</f>
+        <v>0.91900000000000004</v>
+      </c>
+      <c r="E7" s="245">
+        <f>+Final!AK18</f>
+        <v>0.90400000000000003</v>
+      </c>
+      <c r="F7" s="245">
+        <f>1-(+E7/D7)</f>
+        <v>1.6322089227421177E-2</v>
+      </c>
+      <c r="G7" s="250">
+        <f>+Final!AJ20</f>
+        <v>0.93899999999999995</v>
+      </c>
+      <c r="H7" s="251">
+        <f>+Final!AK20</f>
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="I7" s="256">
+        <f>1-(+H7/G7)</f>
+        <v>1.1714589989350266E-2</v>
+      </c>
+      <c r="J7" s="244">
+        <f>+Final!AJ23</f>
+        <v>0.96</v>
+      </c>
+      <c r="K7" s="245">
+        <f>+Final!AK23</f>
+        <v>0.93</v>
+      </c>
+      <c r="L7" s="246">
+        <f>1-(+K7/J7)</f>
+        <v>3.1249999999999889E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C8" s="235" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="247" t="s">
+        <v>79</v>
+      </c>
+      <c r="E8" s="248" t="s">
+        <v>79</v>
+      </c>
+      <c r="F8" s="249" t="s">
+        <v>79</v>
+      </c>
+      <c r="G8" s="247" t="s">
+        <v>79</v>
+      </c>
+      <c r="H8" s="248" t="s">
+        <v>79</v>
+      </c>
+      <c r="I8" s="249" t="s">
+        <v>79</v>
+      </c>
+      <c r="J8" s="257">
+        <f>+Final!AL23</f>
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="K8" s="252">
+        <f>+Final!AM23</f>
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="L8" s="253">
+        <f>1-(+K8/J8)</f>
+        <v>4.8533872598584438E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:I3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>